<commit_message>
commiting ECR approval for end to test
</commit_message>
<xml_diff>
--- a/Data Files/BEP/TestDataEstimate.xlsx
+++ b/Data Files/BEP/TestDataEstimate.xlsx
@@ -5730,9 +5730,6 @@
     <t>brads@pegasystems.com</t>
   </si>
   <si>
-    <t>winth@pegasystems.com</t>
-  </si>
-  <si>
     <t>stafc@pegasystems.com</t>
   </si>
   <si>
@@ -5743,13 +5740,16 @@
   </si>
   <si>
     <t>BEP-01Apr2018-14</t>
+  </si>
+  <si>
+    <t>meack@pegasystems.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5777,6 +5777,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5841,12 +5849,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -5861,10 +5870,12 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6145,8 +6156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6216,7 +6227,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -6234,11 +6245,11 @@
       <c r="H2" s="1" t="s">
         <v>1881</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="8" t="s">
+        <v>1904</v>
+      </c>
+      <c r="J2" t="s">
         <v>1900</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1901</v>
       </c>
       <c r="K2" t="s">
         <v>1892</v>
@@ -6258,7 +6269,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
@@ -6277,10 +6288,10 @@
         <v>1893</v>
       </c>
       <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
         <v>1900</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1901</v>
       </c>
       <c r="K3" t="s">
         <v>1882</v>
@@ -6417,16 +6428,17 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1"/>
     <hyperlink ref="N3:N6" r:id="rId2" display="diazz@pegasystems.com"/>
+    <hyperlink ref="I2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>